<commit_message>
Shikun Xiong Diary update (#84)
* Team 8 project update

Team 8 claims lombok as the team project

* shikun Xiong Diary update

* Update projects.md

* Update diary-Shikun Xiong.xlsx

* Update diary-Shikun Xiong.xlsx

* Update diary-Shikun Xiong.xlsx

* Update diary-Shikun Xiong.xlsx
</commit_message>
<xml_diff>
--- a/diaries/diary-Shikun Xiong.xlsx
+++ b/diaries/diary-Shikun Xiong.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -131,6 +131,21 @@
   </si>
   <si>
     <t>Not bad</t>
+  </si>
+  <si>
+    <t>Change the team project to a more suitable one</t>
+  </si>
+  <si>
+    <t>I just think that last project is not that appropriate. Anyway, I find another Android app since we can run it and see the features, it's easier and more interesting to explore this project.</t>
+  </si>
+  <si>
+    <t>1/18/2020</t>
+  </si>
+  <si>
+    <t>Finish the assignment</t>
+  </si>
+  <si>
+    <t>It's interesting to explore the Pacman project. I did just what we learnt on class, it's really useful.</t>
   </si>
 </sst>
 </file>
@@ -138,8 +153,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
@@ -236,6 +251,82 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -245,16 +336,25 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="134"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -265,91 +365,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -378,169 +393,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -556,39 +571,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -610,29 +597,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -651,16 +618,64 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -669,14 +684,14 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -685,111 +700,111 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1152,8 +1167,8 @@
   <sheetPr/>
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="6"/>
@@ -1385,23 +1400,51 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" ht="15.6" spans="1:7">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="12"/>
-    </row>
-    <row r="16" ht="15.6" spans="1:7">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="12"/>
+    <row r="15" ht="102" customHeight="1" spans="1:7">
+      <c r="A15" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="11">
+        <v>0.925694444444444</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" ht="64" customHeight="1" spans="1:7">
+      <c r="A16" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="11">
+        <v>0.518055555555556</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="17" ht="15.6" spans="1:7">
       <c r="A17" s="9"/>

</xml_diff>

<commit_message>
Update diary-Shikun Xiong.xlsx (#255)
</commit_message>
<xml_diff>
--- a/diaries/diary-Shikun Xiong.xlsx
+++ b/diaries/diary-Shikun Xiong.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="81">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -218,6 +218,45 @@
   </si>
   <si>
     <t>We reviewed the assignment this morning and submit it.</t>
+  </si>
+  <si>
+    <t>1/31/2020</t>
+  </si>
+  <si>
+    <t>Review the course, and prepare for the assignments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The features our team find last time are definitely not essential features. I thought that the Maintable in our project is an essential feature, but how to define the boundary of this feature might be a problem. </t>
+  </si>
+  <si>
+    <t>2/2/2020</t>
+  </si>
+  <si>
+    <t>Discuss the assignments</t>
+  </si>
+  <si>
+    <t>Our team decides to have a team discussion next week. I want to prepare something for the discussion, so I try to find some clues about the feature "Maintable"</t>
+  </si>
+  <si>
+    <t>2/4/2020</t>
+  </si>
+  <si>
+    <t>Team discussion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We had the team discussion this afternoon, and divided tasks to different members. Although we had some divergence, we have agreement in the end. We set the MainTable and EntryEditor as our two features. Besides, we want to explain the MainTable in a kind of high level and EntryEditor in details. </t>
+  </si>
+  <si>
+    <t>2/5/2020</t>
+  </si>
+  <si>
+    <t>Do assignments</t>
+  </si>
+  <si>
+    <t>Almost done</t>
+  </si>
+  <si>
+    <t>We discussed a lot of things about the assignment, such as the format, what kind of diagram we need, etc. We add more things to our assignment, it's almost done.</t>
   </si>
 </sst>
 </file>
@@ -225,10 +264,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -324,6 +363,74 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -340,76 +447,8 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -423,18 +462,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -445,6 +476,14 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -473,13 +512,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -491,7 +590,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -503,133 +632,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -673,11 +712,61 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -696,66 +785,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -764,14 +803,14 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -780,111 +819,111 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="32" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1248,8 +1287,8 @@
   <sheetPr/>
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E21" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="6"/>
@@ -1688,41 +1727,97 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" ht="15.6" spans="1:7">
-      <c r="A24" s="11"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="13"/>
-    </row>
-    <row r="25" ht="15.6" spans="1:7">
-      <c r="A25" s="11"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="13"/>
-    </row>
-    <row r="26" ht="15.6" spans="1:7">
-      <c r="A26" s="11"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="13"/>
-    </row>
-    <row r="27" ht="15.6" spans="1:7">
-      <c r="A27" s="11"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="13"/>
+    <row r="24" ht="115" customHeight="1" spans="1:7">
+      <c r="A24" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="12">
+        <v>0.5375</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" ht="100" customHeight="1" spans="1:7">
+      <c r="A25" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" s="12">
+        <v>0.891666666666667</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" ht="164" customHeight="1" spans="1:7">
+      <c r="A26" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" s="12">
+        <v>0.954166666666667</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" ht="99" customHeight="1" spans="1:7">
+      <c r="A27" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" s="12">
+        <v>0.625</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="28" ht="15.6" spans="1:7">
       <c r="A28" s="11"/>

</xml_diff>

<commit_message>
Update diary-Shikun Xiong.xlsx (#337)
</commit_message>
<xml_diff>
--- a/diaries/diary-Shikun Xiong.xlsx
+++ b/diaries/diary-Shikun Xiong.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="105">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -287,6 +287,48 @@
   </si>
   <si>
     <t>Bad</t>
+  </si>
+  <si>
+    <t>2/13/2020</t>
+  </si>
+  <si>
+    <t>Review the slides</t>
+  </si>
+  <si>
+    <t>Today I think I have learnt something outside the codes. It makes me realize that people related to the project, such as stakeholder, developers, are also important for a project</t>
+  </si>
+  <si>
+    <t>2/16/2020</t>
+  </si>
+  <si>
+    <t>Revise the assignment2</t>
+  </si>
+  <si>
+    <t>We found a new feature for assignment2. But there are still a lot of things left to finish.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Since this week we talked to Kaj, he taught us a lot of things about report. Especially how to relate the diagrams to text, how to make report concise. </t>
+  </si>
+  <si>
+    <t>2/17/2020</t>
+  </si>
+  <si>
+    <t>Add more stuff to the new feature and revise the feature2.</t>
+  </si>
+  <si>
+    <t>When I look to our feature2 again, I find some places to improve. For example. I add a little more explanation to the diagram. What I can learn from this is that always consider yourself as a reader, could you totally understand this report?</t>
+  </si>
+  <si>
+    <t>2/18/2020</t>
+  </si>
+  <si>
+    <t>Start assignment3</t>
+  </si>
+  <si>
+    <t>We divide the assignment to three parts, each team member has one.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I find out that I don't totally understand what's the stakeholders in our project. I still need more time on it. </t>
   </si>
 </sst>
 </file>
@@ -295,8 +337,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
@@ -393,14 +435,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="等线"/>
@@ -408,28 +442,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
@@ -445,8 +457,77 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -461,59 +542,20 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -542,37 +584,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -584,127 +740,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -715,32 +757,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -764,15 +780,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -815,16 +822,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -833,14 +875,14 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -849,111 +891,111 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="29" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1317,8 +1359,8 @@
   <sheetPr/>
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="6"/>
@@ -1918,41 +1960,97 @@
         <v>90</v>
       </c>
     </row>
-    <row r="31" ht="15.6" spans="1:7">
-      <c r="A31" s="11"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="13"/>
-    </row>
-    <row r="32" ht="15.6" spans="1:7">
-      <c r="A32" s="11"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="13"/>
-    </row>
-    <row r="33" ht="15.6" spans="1:7">
-      <c r="A33" s="11"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="13"/>
-    </row>
-    <row r="34" ht="15.6" spans="1:7">
-      <c r="A34" s="11"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="13"/>
+    <row r="31" ht="109" customHeight="1" spans="1:7">
+      <c r="A31" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B31" s="12">
+        <v>0.993055555555556</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" ht="89" customHeight="1" spans="1:7">
+      <c r="A32" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B32" s="12">
+        <v>0.536111111111111</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" ht="123" customHeight="1" spans="1:7">
+      <c r="A33" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B33" s="12">
+        <v>0.895138888888889</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" ht="85" customHeight="1" spans="1:7">
+      <c r="A34" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B34" s="12">
+        <v>0.966666666666667</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="G34" s="13" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="35" ht="15.6" spans="1:7">
       <c r="A35" s="11"/>

</xml_diff>

<commit_message>
Shikun Xiong Diary updated (#404)
* Update diary-Shikun Xiong.xlsx

* Create hw3_C#-er_than_you.pdf

* resubmit hm2

* Update diary-Shikun Xiong.xlsx
</commit_message>
<xml_diff>
--- a/diaries/diary-Shikun Xiong.xlsx
+++ b/diaries/diary-Shikun Xiong.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="118">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -329,6 +329,45 @@
   </si>
   <si>
     <t xml:space="preserve">I find out that I don't totally understand what's the stakeholders in our project. I still need more time on it. </t>
+  </si>
+  <si>
+    <t>2/20/2020</t>
+  </si>
+  <si>
+    <t>find interesting issues for our project</t>
+  </si>
+  <si>
+    <t>almost done</t>
+  </si>
+  <si>
+    <t>This task is kind of difficult since I am not sure how to define "interesting". I spent a long time reading the issues one by one, however, the process itself it's interesting. I saw people have different ideas about this same project, and everyone met different problems.</t>
+  </si>
+  <si>
+    <t>2/21/2020</t>
+  </si>
+  <si>
+    <t>find 5 interesting issues</t>
+  </si>
+  <si>
+    <t>I did find something interesting. Those people are really humorous. After this assginment, I just realize that looking through issues is not that boring.</t>
+  </si>
+  <si>
+    <t>2/22/2020</t>
+  </si>
+  <si>
+    <t>discuss the architecture</t>
+  </si>
+  <si>
+    <t>We find some documentions about the architecture. But we think we can still draw our own. I get to know that architecture should be clear and concise, we don't need something complex.</t>
+  </si>
+  <si>
+    <t>2/24/2020</t>
+  </si>
+  <si>
+    <t>draw architecture for project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We draw the diagrams today and attach some explanations. This really helps us better understand the whole project. I just feel that we should have done this at the very beginning, because this is really helpful. </t>
   </si>
 </sst>
 </file>
@@ -338,8 +377,8 @@
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -435,6 +474,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="等线"/>
@@ -444,6 +498,28 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -465,55 +541,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -535,27 +575,26 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -584,163 +623,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -762,9 +801,59 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -780,21 +869,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -822,51 +896,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -875,14 +914,14 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -891,111 +930,111 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1359,8 +1398,8 @@
   <sheetPr/>
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="6"/>
@@ -2052,41 +2091,97 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" ht="15.6" spans="1:7">
-      <c r="A35" s="11"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="13"/>
-    </row>
-    <row r="36" ht="15.6" spans="1:7">
-      <c r="A36" s="11"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="13"/>
-    </row>
-    <row r="37" ht="15.6" spans="1:7">
-      <c r="A37" s="11"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="13"/>
-    </row>
-    <row r="38" ht="15.6" spans="1:7">
-      <c r="A38" s="11"/>
-      <c r="B38" s="11"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="13"/>
+    <row r="35" ht="153" customHeight="1" spans="1:7">
+      <c r="A35" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B35" s="12">
+        <v>0.995138888888889</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="G35" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" ht="100" customHeight="1" spans="1:7">
+      <c r="A36" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B36" s="12">
+        <v>0.805555555555556</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="G36" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" ht="97" customHeight="1" spans="1:7">
+      <c r="A37" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B37" s="12">
+        <v>0.8625</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="F37" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="G37" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" ht="134" customHeight="1" spans="1:7">
+      <c r="A38" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B38" s="12">
+        <v>0.890277777777778</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="G38" s="13" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="39" ht="15.6" spans="1:7">
       <c r="A39" s="11"/>

</xml_diff>